<commit_message>
create admin view scenes
</commit_message>
<xml_diff>
--- a/plantilla/datos.xlsx
+++ b/plantilla/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEMPORAL-STALYN\IOT\Clientes\1722439120_Stalyn_Quishpe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7765567-9EF9-4089-8A78-3710BAB7EDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28064657-8EF2-4A72-8E10-ACBE369FDC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="12" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="156">
   <si>
     <t>domain</t>
   </si>
@@ -567,6 +567,9 @@
   </si>
   <si>
     <t>SWITCH_VALUES</t>
+  </si>
+  <si>
+    <t>orden_view</t>
   </si>
 </sst>
 </file>
@@ -1022,8 +1025,8 @@
   </sheetPr>
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2426,100 +2429,119 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B077E1-37B3-4FBB-9A26-0E96A61E0B94}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>146</v>
-      </c>
-      <c r="C2" t="s">
-        <v>144</v>
       </c>
       <c r="D2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="16">
+        <v>2</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>147</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="16">
+        <v>3</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>148</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="16">
+        <v>4</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="16">
+        <v>5</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>144</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2532,7 +2554,7 @@
           <x14:formula1>
             <xm:f>'Datos ComboBox'!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:D6</xm:sqref>
+          <xm:sqref>D2:E6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Creacion de grupos genericos por zona
</commit_message>
<xml_diff>
--- a/plantilla/datos.xlsx
+++ b/plantilla/datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEMPORAL-STALYN\IOT\Clientes\1722439120_Stalyn_Quishpe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0862185A-C4A5-4F63-9F53-9C960B5A0D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DCB225-D6A4-4DE1-BE05-9DD429D4128A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Entidades!$B$1:$V$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -213,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="181">
   <si>
     <t>domain</t>
   </si>
@@ -699,9 +698,6 @@
     <t>orden_view</t>
   </si>
   <si>
-    <t>Luz_directa</t>
-  </si>
-  <si>
     <t>POSICION_EN_VIEW</t>
   </si>
   <si>
@@ -766,6 +762,18 @@
   </si>
   <si>
     <t>Bateria_Sensor_TH</t>
+  </si>
+  <si>
+    <t>create_card_temperature_and_humedity_sensor</t>
+  </si>
+  <si>
+    <t>Luz directa</t>
+  </si>
+  <si>
+    <t>Motor-Cortina</t>
+  </si>
+  <si>
+    <t>M_Cortina</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1238,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2245,7 +2253,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>77</v>
@@ -2264,31 +2272,31 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="0"/>
-        <v>switch.interruptor_doble_pared_luz_directa_01_zigbee_01_interior_sala</v>
+        <v>switch.interruptor_doble_pared_luz directa_01_zigbee_01_interior_sala</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" si="1"/>
-        <v>Interruptor_doble_Luz_directa_01_zigbee_01_Sala_Interior</v>
+        <v>Interruptor_doble_Luz directa_01_zigbee_01_Sala_Interior</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="2"/>
-        <v>Sala_Interior_Interruptor_doble_01_Luz_directa</v>
+        <v>Sala_Interior_Interruptor_doble_01_Luz directa</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" si="3"/>
-        <v>01  Luz_directa de la Sala</v>
+        <v>01  Luz directa de la Sala</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="4"/>
-        <v>Casa/Interior/Segunda-planta/Sala/switch/Interruptor-doble/01/Luz_directa/</v>
+        <v>Casa/Interior/Segunda-planta/Sala/switch/Interruptor-doble/01/Luz directa/</v>
       </c>
       <c r="T14" t="str">
         <f t="shared" si="5"/>
-        <v>Interruptor-doble_01_Luz_directa_de_la_Sala</v>
+        <v>Interruptor-doble_01_Luz directa_de_la_Sala</v>
       </c>
       <c r="U14" t="str">
         <f t="shared" si="6"/>
-        <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Sala/Interruptor-doble_01_Luz_directa_de_la_Sala.svg</v>
+        <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Sala/Interruptor-doble_01_Luz directa_de_la_Sala.svg</v>
       </c>
       <c r="V14" s="4" t="s">
         <v>10</v>
@@ -2339,31 +2347,31 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
-        <v>sensor.sensor_pared_temperatura_00_zigbee_01_interior_sala</v>
+        <v>sensor.sensor_pared_humedad_00_zigbee_01_interior_sala</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="1"/>
-        <v>Sensor_Temperatura_00_zigbee_01_Sala_Interior</v>
+        <v>Sensor_Humedad_00_zigbee_01_Sala_Interior</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="2"/>
-        <v>Sala_Interior_Sensor_00_Temperatura</v>
+        <v>Sala_Interior_Sensor_00_Humedad</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> Temperatura de la Sala</v>
+        <v xml:space="preserve"> Humedad de la Sala</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="4"/>
-        <v>Casa/Interior/Segunda-planta/Sala/sensor/Sensor/00/Temperatura/</v>
+        <v>Casa/Interior/Segunda-planta/Sala/sensor/Sensor/00/Humedad/</v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="5"/>
-        <v>Sensor_Temperatura_de_la_Sala</v>
+        <v>Sensor_Humedad_de_la_Sala</v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="6"/>
-        <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Sala/Sensor_Temperatura_de_la_Sala.svg</v>
+        <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Sala/Sensor_Humedad_de_la_Sala.svg</v>
       </c>
       <c r="V15" s="4" t="s">
         <v>10</v>
@@ -2395,7 +2403,7 @@
         <v>8</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>77</v>
@@ -2414,31 +2422,31 @@
       </c>
       <c r="O16" t="str">
         <f t="shared" si="0"/>
-        <v>sensor.sensor_pared_humedad_00_zigbee_01_interior_sala</v>
+        <v>sensor.sensor_pared_temperatura_00_zigbee_01_interior_sala</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="1"/>
-        <v>Sensor_Humedad_00_zigbee_01_Sala_Interior</v>
+        <v>Sensor_Temperatura_00_zigbee_01_Sala_Interior</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="2"/>
-        <v>Sala_Interior_Sensor_00_Humedad</v>
+        <v>Sala_Interior_Sensor_00_Temperatura</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> Humedad de la Sala</v>
+        <v xml:space="preserve"> Temperatura de la Sala</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="4"/>
-        <v>Casa/Interior/Segunda-planta/Sala/sensor/Sensor/00/Humedad/</v>
+        <v>Casa/Interior/Segunda-planta/Sala/sensor/Sensor/00/Temperatura/</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="5"/>
-        <v>Sensor_Humedad_de_la_Sala</v>
+        <v>Sensor_Temperatura_de_la_Sala</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="6"/>
-        <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Sala/Sensor_Humedad_de_la_Sala.svg</v>
+        <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Sala/Sensor_Temperatura_de_la_Sala.svg</v>
       </c>
       <c r="V16" s="4" t="s">
         <v>10</v>
@@ -2470,7 +2478,7 @@
         <v>8</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>77</v>
@@ -2516,6 +2524,81 @@
         <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Sala/Sensor_Bateria_Sensor_TH_de_la_Sala.svg</v>
       </c>
       <c r="V17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" ref="O18" si="7">LOWER(SUBSTITUTE(CONCATENATE(F18,".",G18,V18,E18,V18,I18,V18,H18,V18,J18,V18,LEFT(K18,2),V18,B18,V18,D18),"-","_"))</f>
+        <v>cover.motor_cortina_pared_m_cortina_00_zigbee_01_interior_estudio</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" ref="P18" si="8">SUBSTITUTE(CONCATENATE(G18,V18,I18,V18,H18,V18,J18,V18,LEFT(K18,2),V18,D18,V18,B18),"-","_")</f>
+        <v>Motor_Cortina_M_Cortina_00_zigbee_01_Estudio_Interior</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" ref="Q18" si="9">SUBSTITUTE(CONCATENATE((D18),V18,(B18),V18,(G18),V18,H18, V18, I18),"-","_")</f>
+        <v>Estudio_Interior_Motor_Cortina_00_M_Cortina</v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" ref="R18" si="10">SUBSTITUTE(CONCATENATE(IF(H18="00",,CONCATENATE(H18," "))," ",I18," ",N18," ",D18),"-", " ")</f>
+        <v xml:space="preserve"> M_Cortina del Estudio</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" ref="S18" si="11">_xlfn.CONCAT(A18,"/",B18,"/",C18,"/",D18,"/",F18,"/",G18,"/",H18,"/",I18,"/")</f>
+        <v>Casa/Interior/Segunda-planta/Estudio/cover/Motor-Cortina/00/M_Cortina/</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" ref="T18" si="12">CONCATENATE(G18,V18,IF(H18="00",,CONCATENATE(H18,V18)),I18,V18,SUBSTITUTE(N18," ","_"),V18,D18)</f>
+        <v>Motor-Cortina_M_Cortina_del_Estudio</v>
+      </c>
+      <c r="U18" t="str">
+        <f t="shared" ref="U18" si="13">_xlfn.CONCAT("/local/ismart/planos/Zonas/",B18,"/Ubicacion","/",C18,"/Areas","/",D18,"/",T18,".svg")</f>
+        <v>/local/ismart/planos/Zonas/Interior/Ubicacion/Segunda-planta/Areas/Estudio/Motor-Cortina_M_Cortina_del_Estudio.svg</v>
+      </c>
+      <c r="V18" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2534,11 +2617,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39826518-181E-4705-8E10-895592D5D3B6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{820B1DE8-0DFF-43CE-87BC-815AA122B86A}">
           <x14:formula1>
-            <xm:f>AreasSK!$A$2:$A$32</xm:f>
+            <xm:f>AreasSK!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>D9:D17</xm:sqref>
+          <xm:sqref>D8 D10:D11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D45CE4A7-E42B-4756-998A-3C7CEDAE1670}">
           <x14:formula1>
@@ -2546,59 +2629,59 @@
           </x14:formula1>
           <xm:sqref>D2:D7</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39826518-181E-4705-8E10-895592D5D3B6}">
+          <x14:formula1>
+            <xm:f>AreasSK!$A$2:$A$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>D9:D18</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E9886CA0-ABF7-4DEF-981A-938147170D13}">
           <x14:formula1>
             <xm:f>Zona!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B17</xm:sqref>
+          <xm:sqref>B2:B18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D7E912A-9EEA-4A7E-BA71-EB1AE0E4ADA5}">
           <x14:formula1>
-            <xm:f>Type!$A$2:$A$22</xm:f>
+            <xm:f>Type!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G17</xm:sqref>
+          <xm:sqref>G2:G18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CBB5A09-5E5C-407E-BA26-A7699A10D719}">
           <x14:formula1>
             <xm:f>LocationDevice!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E17</xm:sqref>
+          <xm:sqref>E2:E18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{46FF9668-8E5B-4F69-99AC-869AA36609B8}">
           <x14:formula1>
             <xm:f>Ubicacion!$A$2:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C17</xm:sqref>
+          <xm:sqref>C2:C18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E02A4412-B018-4DF2-8E88-469CB105D9E7}">
           <x14:formula1>
             <xm:f>Technology!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J17</xm:sqref>
+          <xm:sqref>J2:J18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00765230-EFF7-4A9F-8655-D4A0D5B527BE}">
           <x14:formula1>
             <xm:f>Importance!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{820B1DE8-0DFF-43CE-87BC-815AA122B86A}">
-          <x14:formula1>
-            <xm:f>AreasSK!$A$2:$A$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>D8 D10:D11</xm:sqref>
+          <xm:sqref>K2:K18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60A29141-6D71-45D0-B030-450CD38D68A6}">
           <x14:formula1>
-            <xm:f>Nombre_Entidades!$A$2:$A$7</xm:f>
+            <xm:f>Nombre_Entidades!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I17</xm:sqref>
+          <xm:sqref>I2:I18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DE8FA183-60B6-45C4-9BE0-181207916F32}">
           <x14:formula1>
             <xm:f>Domain!$A$2:$A$28</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F17</xm:sqref>
+          <xm:sqref>F2:F18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2700,7 +2783,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD521F66-7339-4766-87AE-20EB5EAC51B7}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -2728,24 +2811,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="16" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" s="26"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="16" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2757,8 +2845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6369E091-0E04-40BB-909D-8136BCC61440}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2767,7 +2855,7 @@
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="22.25" customWidth="1"/>
     <col min="5" max="5" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.5" customWidth="1"/>
+    <col min="7" max="7" width="52.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15">
@@ -2784,10 +2872,10 @@
         <v>153</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2804,10 +2892,10 @@
         <v>143</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2824,10 +2912,10 @@
         <v>144</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2837,10 +2925,10 @@
       <c r="C4" s="26"/>
       <c r="D4" s="16"/>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2849,7 +2937,7 @@
       </c>
       <c r="D5" s="16"/>
       <c r="G5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2858,18 +2946,22 @@
       </c>
       <c r="D6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="25" t="s">
         <v>103</v>
       </c>
+      <c r="G7" s="16" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" s="25" t="s">
         <v>104</v>
       </c>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" s="25" t="s">
@@ -3179,7 +3271,7 @@
         <v>101</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" t="s">
         <v>95</v>
@@ -3196,7 +3288,7 @@
         <v>100</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
         <v>95</v>
@@ -3213,7 +3305,7 @@
         <v>106</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" t="s">
         <v>96</v>
@@ -3230,7 +3322,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s">
         <v>95</v>
@@ -3627,10 +3719,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3643,33 +3735,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15">
       <c r="A1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="21" t="s">
-        <v>165</v>
-      </c>
       <c r="F1" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
         <v>135</v>
@@ -3678,19 +3770,19 @@
         <v>37</v>
       </c>
       <c r="F2" t="str">
-        <f>_xlfn.CONCAT(A2,"~",E2)</f>
+        <f t="shared" ref="F2:F11" si="0">_xlfn.CONCAT(A2,"~",E2)</f>
         <v>create_card_title_welcome_smart~Cocina</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
@@ -3699,19 +3791,19 @@
         <v>37</v>
       </c>
       <c r="F3" t="str">
-        <f>_xlfn.CONCAT(A3,"~",E3)</f>
+        <f t="shared" si="0"/>
         <v>create_card_scenes_welcome~Cocina</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>168</v>
+      <c r="A4" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" t="s">
         <v>135</v>
@@ -3720,19 +3812,19 @@
         <v>37</v>
       </c>
       <c r="F4" t="str">
-        <f>_xlfn.CONCAT(A4,"~",E4)</f>
+        <f t="shared" si="0"/>
         <v>card_group_switch_entities~Cocina</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" t="s">
         <v>135</v>
@@ -3741,19 +3833,19 @@
         <v>37</v>
       </c>
       <c r="F5" t="str">
-        <f>_xlfn.CONCAT(A5,"~",E5)</f>
+        <f t="shared" si="0"/>
         <v>create_card_clock~Cocina</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D6" t="s">
         <v>135</v>
@@ -3762,46 +3854,151 @@
         <v>37</v>
       </c>
       <c r="F6" t="str">
-        <f>_xlfn.CONCAT(A6,"~",E6)</f>
+        <f t="shared" si="0"/>
         <v>create_card_list_of_notes~Cocina</v>
       </c>
     </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>create_card_title_welcome_smart~Sala</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>create_card_temperature_and_humedity_sensor~Sala</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>create_card_clock~Sala</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>create_card_scenes_welcome~Sala</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>card_group_switch_entities~Sala</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F8:F1048576 F1:F6">
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro repedito" error="Hay registros repetidos_x000a_en las columnas_x000a_name_cards_i_ismar y order" sqref="B2:B5 B6" xr:uid="{37AE49D2-9CED-4E6E-9EBC-C46311551CD2}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro repedito" error="Hay registros repetidos_x000a_en las columnas_x000a_name_cards_i_ismar y order" sqref="B2:B11" xr:uid="{37AE49D2-9CED-4E6E-9EBC-C46311551CD2}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro repedito" error="Hay registros repetidos_x000a_en las columnas_x000a_name_cards_i_ismar y order" xr:uid="{F02249E7-15AC-41DC-8A5E-CC9ECC2BC7BD}">
           <x14:formula1>
             <xm:f>'Datos ComboBox'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D5 D6</xm:sqref>
+          <xm:sqref>D2:D11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro repedito" error="Hay registros repetidos_x000a_en las columnas_x000a_name_cards_i_ismar y order" xr:uid="{E5F6FFA7-9561-46C7-8026-03E748D14487}">
           <x14:formula1>
             <xm:f>AreasSK!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E5 E6</xm:sqref>
+          <xm:sqref>E2:E11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro repedito" error="Hay registros repetidos_x000a_en las columnas_x000a_name_cards_i_ismar y order" xr:uid="{C5473ADE-DC07-49B2-A82F-62EEC8FC8C54}">
           <x14:formula1>
             <xm:f>'Datos ComboBox'!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C5 C6</xm:sqref>
+          <xm:sqref>C2:C11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro repedito" error="Hay registros repetidos_x000a_en las columnas_x000a_name_cards_i_ismar y order" xr:uid="{7986FA5B-1C52-49BD-98F6-A9B7A99D71BA}">
           <x14:formula1>
-            <xm:f>'Datos ComboBox'!$G$2:$G$6</xm:f>
+            <xm:f>'Datos ComboBox'!$G$2:$G$7</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A5 A6</xm:sqref>
+          <xm:sqref>A2:A11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3952,10 +4149,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C995BE-9AFD-4F24-9038-2BC0697FD49C}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -4011,6 +4208,11 @@
     <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="16" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generacion de archivos configuration.yaml
</commit_message>
<xml_diff>
--- a/plantilla/datos.xlsx
+++ b/plantilla/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TEMPORAL-STALYN\IOT\Clientes\1722439120_Stalyn_Quishpe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390587F-0E82-40C1-BE14-BAB597D3957F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B196A062-8AF2-47A2-BDE3-6B9D4291AC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuracion" sheetId="21" r:id="rId1"/>
@@ -978,7 +978,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1024,31 +1024,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1096,6 +1081,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1316,7 +1308,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1351,7 +1343,7 @@
       <c r="A3" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>189</v>
       </c>
       <c r="C3" s="23" t="s">
@@ -1362,7 +1354,7 @@
       <c r="A4" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>200</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1376,7 +1368,7 @@
       <c r="B5" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="23" t="s">
@@ -1390,25 +1382,20 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="23" t="s">
         <v>195</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B6">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B2:B7">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(B2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3392,7 +3379,7 @@
     <sortCondition ref="B2:B16"/>
   </sortState>
   <conditionalFormatting sqref="O20:O1048576 O1:O18">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3756,15 +3743,15 @@
   </sortState>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B16">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C15">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3809,42 +3796,42 @@
       <c r="A1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="16" t="s">
@@ -4258,7 +4245,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro repedito" error="Hay registros repetidos_x000a_en las columnas_x000a_name_cards_i_ismar y order" sqref="B2:B14" xr:uid="{37AE49D2-9CED-4E6E-9EBC-C46311551CD2}"/>

</xml_diff>